<commit_message>
add atividades colaborativas e individual
</commit_message>
<xml_diff>
--- a/REGRAS.xlsx
+++ b/REGRAS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dimensão 1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="43">
   <si>
     <t>1. as VA utilizaram slides com textos e imagens que favoreceram a aprendizagem.</t>
   </si>
@@ -303,9 +303,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -336,14 +338,16 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Saída" xfId="1" builtinId="21"/>
   </cellStyles>
@@ -646,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -659,27 +663,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -964,7 +968,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>9</v>
@@ -1276,11 +1280,11 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
@@ -1933,40 +1937,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E73" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="106.5" customWidth="1"/>
-    <col min="4" max="4" width="106" customWidth="1"/>
+    <col min="1" max="1" width="76.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="72.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1994,55 +2000,75 @@
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
@@ -2070,55 +2096,75 @@
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
@@ -2146,55 +2192,75 @@
       <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
@@ -2222,55 +2288,75 @@
       <c r="A30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="9"/>
+      <c r="E34" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
@@ -2298,55 +2384,79 @@
       <c r="A38" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="5"/>
+      <c r="B40" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C40" s="2"/>
       <c r="D40" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="5"/>
+      <c r="B41" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="E41" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="9"/>
+      <c r="B42" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="9"/>
+      <c r="E42" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B43" s="9"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -2374,56 +2484,77 @@
       <c r="A46" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="5"/>
+      <c r="B46" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C46" s="2"/>
       <c r="D46" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="5"/>
+      <c r="B47" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C47" s="2"/>
       <c r="D47" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C48" s="2"/>
       <c r="D48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="E48" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C49" s="2"/>
       <c r="D49" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="9"/>
+      <c r="B50" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="9"/>
-    </row>
+      <c r="E50" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>10</v>
@@ -2450,55 +2581,75 @@
       <c r="A54" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="5"/>
+      <c r="B54" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C54" s="2"/>
       <c r="D54" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="5"/>
+      <c r="B55" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C55" s="2"/>
       <c r="D55" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="5"/>
+      <c r="E55" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="5"/>
+      <c r="B56" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C56" s="2"/>
       <c r="D56" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="5"/>
+      <c r="B57" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C57" s="2"/>
       <c r="D57" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E57" s="5"/>
+      <c r="E57" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="9"/>
+      <c r="B58" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D58" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E58" s="9"/>
+      <c r="E58" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
@@ -2526,55 +2677,75 @@
       <c r="A62" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="5"/>
+      <c r="B62" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E62" s="5"/>
+      <c r="E62" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C63" s="2"/>
       <c r="D63" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E63" s="5"/>
+      <c r="E63" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="5"/>
+      <c r="B64" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C64" s="2"/>
       <c r="D64" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E64" s="5"/>
+      <c r="E64" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="5"/>
+      <c r="B65" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C65" s="2"/>
       <c r="D65" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E65" s="5"/>
+      <c r="E65" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B66" s="9"/>
+      <c r="B66" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D66" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E66" s="9"/>
+      <c r="E66" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
@@ -2602,55 +2773,75 @@
       <c r="A70" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B70" s="5"/>
+      <c r="B70" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C70" s="2"/>
       <c r="D70" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="5"/>
+      <c r="E70" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="5"/>
+      <c r="B71" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C71" s="2"/>
       <c r="D71" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="5"/>
+      <c r="E71" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B72" s="5"/>
+      <c r="B72" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C72" s="2"/>
       <c r="D72" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E72" s="5"/>
+      <c r="E72" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B73" s="5"/>
+      <c r="B73" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C73" s="2"/>
       <c r="D73" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E73" s="5"/>
+      <c r="E73" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="9"/>
+      <c r="B74" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D74" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E74" s="9"/>
+      <c r="E74" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
@@ -2678,55 +2869,75 @@
       <c r="A78" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B78" s="5"/>
+      <c r="B78" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C78" s="2"/>
       <c r="D78" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E78" s="5"/>
+      <c r="E78" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B79" s="5"/>
+      <c r="B79" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C79" s="2"/>
       <c r="D79" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E79" s="5"/>
+      <c r="E79" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B80" s="5"/>
+      <c r="B80" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C80" s="2"/>
       <c r="D80" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E80" s="5"/>
+      <c r="E80" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="5"/>
+      <c r="B81" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C81" s="2"/>
       <c r="D81" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E81" s="5"/>
+      <c r="E81" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="82" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="9"/>
+      <c r="B82" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D82" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E82" s="9"/>
+      <c r="E82" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="84" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
@@ -2754,55 +2965,75 @@
       <c r="A86" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B86" s="5"/>
+      <c r="B86" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C86" s="2"/>
       <c r="D86" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E86" s="5"/>
+      <c r="E86" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="87" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B87" s="5"/>
+      <c r="B87" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C87" s="2"/>
       <c r="D87" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E87" s="5"/>
+      <c r="E87" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="88" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="5"/>
+      <c r="B88" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C88" s="2"/>
       <c r="D88" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E88" s="5"/>
+      <c r="E88" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B89" s="5"/>
+      <c r="B89" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C89" s="2"/>
       <c r="D89" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E89" s="5"/>
+      <c r="E89" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="9"/>
+      <c r="B90" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D90" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E90" s="9"/>
+      <c r="E90" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
@@ -2830,55 +3061,75 @@
       <c r="A94" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B94" s="5"/>
+      <c r="B94" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C94" s="2"/>
       <c r="D94" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E94" s="5"/>
+      <c r="E94" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B95" s="5"/>
+      <c r="B95" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C95" s="2"/>
       <c r="D95" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E95" s="5"/>
+      <c r="E95" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B96" s="5"/>
+      <c r="B96" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C96" s="2"/>
       <c r="D96" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E96" s="5"/>
+      <c r="E96" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B97" s="5"/>
+      <c r="B97" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C97" s="2"/>
       <c r="D97" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E97" s="5"/>
+      <c r="E97" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B98" s="9"/>
+      <c r="B98" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D98" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E98" s="9"/>
+      <c r="E98" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
@@ -2906,290 +3157,82 @@
       <c r="A102" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B102" s="5"/>
+      <c r="B102" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C102" s="2"/>
       <c r="D102" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E102" s="5"/>
+      <c r="E102" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="103" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B103" s="5"/>
+      <c r="B103" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C103" s="2"/>
       <c r="D103" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E103" s="5"/>
+      <c r="E103" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B104" s="5"/>
+      <c r="B104" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C104" s="2"/>
       <c r="D104" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E104" s="5"/>
+      <c r="E104" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B105" s="5"/>
+      <c r="B105" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C105" s="2"/>
       <c r="D105" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E105" s="5"/>
+      <c r="E105" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B106" s="9"/>
+      <c r="B106" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D106" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E106" s="9"/>
-    </row>
-    <row r="108" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A108" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="7"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="7"/>
-      <c r="E109" s="5"/>
-    </row>
-    <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B110" s="5"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" s="5"/>
-    </row>
-    <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B111" s="5"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E111" s="5"/>
-    </row>
-    <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B112" s="5"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E112" s="5"/>
-    </row>
-    <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A113" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B113" s="5"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E113" s="5"/>
-    </row>
-    <row r="114" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B114" s="9"/>
-      <c r="D114" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E114" s="9"/>
-    </row>
-    <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C116" s="1"/>
-      <c r="D116" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E116" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="7"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="7"/>
-      <c r="E117" s="5"/>
-    </row>
-    <row r="118" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B118" s="5"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E118" s="5"/>
-    </row>
-    <row r="119" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B119" s="5"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E119" s="5"/>
-    </row>
-    <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B120" s="5"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E120" s="5"/>
-    </row>
-    <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A121" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B121" s="5"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E121" s="5"/>
-    </row>
-    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B122" s="9"/>
-      <c r="D122" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E122" s="9"/>
-    </row>
-    <row r="124" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C124" s="1"/>
-      <c r="D124" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E124" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="7"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="7"/>
-      <c r="E125" s="5"/>
-    </row>
-    <row r="126" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B126" s="5"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E126" s="5"/>
-    </row>
-    <row r="127" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B127" s="5"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E127" s="5"/>
-    </row>
-    <row r="128" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A128" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B128" s="5"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E128" s="5"/>
-    </row>
-    <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A129" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B129" s="5"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E129" s="5"/>
-    </row>
-    <row r="130" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A130" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B130" s="9"/>
-      <c r="D130" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E130" s="9"/>
+      <c r="E106" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B10 B38:B42 B86:B90 B102:B106 E102:E106 E6:E10 E86:E90 B14:B18 E14:E18 B22:B26 E38:E42 E22:E26 B30:B34 E30:E34 B46:B50 E46:E50 B54:B58 B110:B114 B70:B74 E54:E58 B62:B66 E62:E66 E70:E74 B78:B82 E78:E82 B94:B98 E110:E114 E94:E98 B118:B122 E118:E122 B126:B130 E126:E130">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:B18 B22:B26 B46:B50 B6:B10 B86:B90 B78:B82 B94:B98 B102:B106 B38:B43 B70:B74 B54:B58 B62:B66 B30:B34 E86:E90 E78:E82 E94:E98 E102:E106 E30:E34 E14:E18 E22:E26 E6:E10 E54:E58 E70:E74 E62:E66 E38:E43 E46:E50">
       <formula1>op</formula1>
     </dataValidation>
   </dataValidations>
@@ -3201,38 +3244,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="106.5" customWidth="1"/>
-    <col min="4" max="4" width="106" customWidth="1"/>
+    <col min="1" max="1" width="76" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="70.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -3260,55 +3304,75 @@
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
@@ -3336,55 +3400,75 @@
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
@@ -3412,55 +3496,75 @@
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
@@ -3488,55 +3592,75 @@
       <c r="A30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="9"/>
+      <c r="E34" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
@@ -3564,55 +3688,79 @@
       <c r="A38" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="5"/>
+      <c r="B40" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C40" s="2"/>
       <c r="D40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="5"/>
+      <c r="B41" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="E41" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="9"/>
+      <c r="B42" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="9"/>
+      <c r="E42" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B43" s="9"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3640,55 +3788,79 @@
       <c r="A46" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="5"/>
+      <c r="B46" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C46" s="2"/>
       <c r="D46" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="5"/>
+      <c r="B47" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C47" s="2"/>
       <c r="D47" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C48" s="2"/>
       <c r="D48" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="E48" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C49" s="2"/>
       <c r="D49" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="9"/>
+      <c r="B50" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="9"/>
+      <c r="E50" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="12"/>
+      <c r="E51" s="12"/>
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
@@ -3716,55 +3888,75 @@
       <c r="A54" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="5"/>
+      <c r="B54" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C54" s="2"/>
       <c r="D54" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="5"/>
+      <c r="B55" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C55" s="2"/>
       <c r="D55" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E55" s="5"/>
+      <c r="E55" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="5"/>
+      <c r="B56" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C56" s="2"/>
       <c r="D56" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="5"/>
+      <c r="B57" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C57" s="2"/>
       <c r="D57" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="5"/>
+      <c r="E57" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="9"/>
+      <c r="B58" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D58" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E58" s="9"/>
+      <c r="E58" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
@@ -3792,55 +3984,75 @@
       <c r="A62" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B62" s="5"/>
+      <c r="B62" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E62" s="5"/>
+      <c r="E62" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C63" s="2"/>
       <c r="D63" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="5"/>
+      <c r="E63" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B64" s="5"/>
+      <c r="B64" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C64" s="2"/>
       <c r="D64" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="5"/>
+      <c r="E64" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="5"/>
+      <c r="B65" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C65" s="2"/>
       <c r="D65" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E65" s="5"/>
+      <c r="E65" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B66" s="9"/>
+      <c r="B66" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D66" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E66" s="9"/>
+      <c r="E66" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
@@ -3868,55 +4080,75 @@
       <c r="A70" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="5"/>
+      <c r="B70" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C70" s="2"/>
       <c r="D70" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="5"/>
+      <c r="E70" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B71" s="5"/>
+      <c r="B71" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C71" s="2"/>
       <c r="D71" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="5"/>
+      <c r="E71" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B72" s="5"/>
+      <c r="B72" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C72" s="2"/>
       <c r="D72" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E72" s="5"/>
+      <c r="E72" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="73" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B73" s="5"/>
+      <c r="B73" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C73" s="2"/>
       <c r="D73" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E73" s="5"/>
+      <c r="E73" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="9"/>
+      <c r="B74" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D74" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E74" s="9"/>
+      <c r="E74" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
@@ -3944,55 +4176,75 @@
       <c r="A78" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B78" s="5"/>
+      <c r="B78" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C78" s="2"/>
       <c r="D78" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="5"/>
+      <c r="E78" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B79" s="5"/>
+      <c r="B79" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C79" s="2"/>
       <c r="D79" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="5"/>
+      <c r="E79" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B80" s="5"/>
+      <c r="B80" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C80" s="2"/>
       <c r="D80" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E80" s="5"/>
+      <c r="E80" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B81" s="5"/>
+      <c r="B81" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C81" s="2"/>
       <c r="D81" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E81" s="5"/>
+      <c r="E81" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="82" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="9"/>
+      <c r="B82" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D82" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E82" s="9"/>
+      <c r="E82" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="84" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
@@ -4020,55 +4272,75 @@
       <c r="A86" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B86" s="5"/>
+      <c r="B86" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C86" s="2"/>
       <c r="D86" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E86" s="5"/>
+      <c r="E86" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="87" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B87" s="5"/>
+      <c r="B87" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C87" s="2"/>
       <c r="D87" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E87" s="5"/>
+      <c r="E87" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="88" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B88" s="5"/>
+      <c r="B88" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C88" s="2"/>
       <c r="D88" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E88" s="5"/>
+      <c r="E88" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="89" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B89" s="5"/>
+      <c r="B89" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C89" s="2"/>
       <c r="D89" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E89" s="5"/>
+      <c r="E89" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="9"/>
+      <c r="B90" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D90" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E90" s="9"/>
+      <c r="E90" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
@@ -4096,55 +4368,75 @@
       <c r="A94" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B94" s="5"/>
+      <c r="B94" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C94" s="2"/>
       <c r="D94" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E94" s="5"/>
+      <c r="E94" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B95" s="5"/>
+      <c r="B95" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C95" s="2"/>
       <c r="D95" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E95" s="5"/>
+      <c r="E95" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B96" s="5"/>
+      <c r="B96" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C96" s="2"/>
       <c r="D96" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E96" s="5"/>
+      <c r="E96" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="97" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B97" s="5"/>
+      <c r="B97" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C97" s="2"/>
       <c r="D97" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E97" s="5"/>
+      <c r="E97" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B98" s="9"/>
+      <c r="B98" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D98" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E98" s="9"/>
+      <c r="E98" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
@@ -4172,290 +4464,256 @@
       <c r="A102" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B102" s="5"/>
+      <c r="B102" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C102" s="2"/>
       <c r="D102" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E102" s="5"/>
+      <c r="E102" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="103" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B103" s="5"/>
+      <c r="B103" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C103" s="2"/>
       <c r="D103" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E103" s="5"/>
+      <c r="E103" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B104" s="5"/>
+      <c r="B104" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C104" s="2"/>
       <c r="D104" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E104" s="5"/>
+      <c r="E104" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="105" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B105" s="5"/>
+      <c r="B105" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C105" s="2"/>
       <c r="D105" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E105" s="5"/>
+      <c r="E105" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B106" s="9"/>
+      <c r="B106" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="D106" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E106" s="9"/>
+      <c r="E106" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="108" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B108" s="8" t="s">
-        <v>2</v>
-      </c>
       <c r="C108" s="1"/>
       <c r="D108" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E108" s="8" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
-      <c r="B109" s="5"/>
       <c r="C109" s="1"/>
       <c r="D109" s="7"/>
-      <c r="E109" s="5"/>
     </row>
     <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B110" s="5"/>
       <c r="C110" s="2"/>
       <c r="D110" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E110" s="5"/>
     </row>
     <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B111" s="5"/>
       <c r="C111" s="2"/>
       <c r="D111" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E111" s="5"/>
     </row>
     <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B112" s="5"/>
       <c r="C112" s="2"/>
       <c r="D112" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E112" s="5"/>
-    </row>
-    <row r="113" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B113" s="5"/>
       <c r="C113" s="2"/>
       <c r="D113" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E113" s="5"/>
-    </row>
-    <row r="114" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B114" s="9"/>
       <c r="D114" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E114" s="9"/>
-    </row>
-    <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>2</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E116" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="7"/>
-      <c r="B117" s="5"/>
       <c r="C117" s="1"/>
       <c r="D117" s="7"/>
-      <c r="E117" s="5"/>
-    </row>
-    <row r="118" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B118" s="5"/>
       <c r="C118" s="2"/>
       <c r="D118" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E118" s="5"/>
-    </row>
-    <row r="119" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B119" s="5"/>
       <c r="C119" s="2"/>
       <c r="D119" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E119" s="5"/>
-    </row>
-    <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B120" s="5"/>
       <c r="C120" s="2"/>
       <c r="D120" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E120" s="5"/>
-    </row>
-    <row r="121" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B121" s="5"/>
       <c r="C121" s="2"/>
       <c r="D121" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E121" s="5"/>
-    </row>
-    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B122" s="9"/>
       <c r="D122" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E122" s="9"/>
-    </row>
-    <row r="124" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>2</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E124" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="7"/>
-      <c r="B125" s="5"/>
       <c r="C125" s="1"/>
       <c r="D125" s="7"/>
-      <c r="E125" s="5"/>
-    </row>
-    <row r="126" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B126" s="5"/>
       <c r="C126" s="2"/>
       <c r="D126" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E126" s="5"/>
-    </row>
-    <row r="127" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B127" s="5"/>
       <c r="C127" s="2"/>
       <c r="D127" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E127" s="5"/>
-    </row>
-    <row r="128" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B128" s="5"/>
       <c r="C128" s="2"/>
       <c r="D128" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E128" s="5"/>
-    </row>
-    <row r="129" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B129" s="5"/>
       <c r="C129" s="2"/>
       <c r="D129" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E129" s="5"/>
-    </row>
-    <row r="130" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B130" s="9"/>
       <c r="D130" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E130" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B10 B38:B42 B22:B26 B70:B74 B86:B90 E6:E10 B14:B18 E22:E26 E14:E18 E70:E74 B78:B82 E86:E90 E78:E82 B94:B98 B30:B34 E30:E34 B54:B58 E94:E98 E38:E42 B46:B50 E54:E58 E46:E50 B62:B66 E62:E66 B102:B106 B118:B122 E102:E106 B110:B114 E118:E122 E110:E114 B126:B130 E126:E130">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B58 B62:B66 B30:B34 B14:B18 B22:B26 B46:B50 B6:B10 B86:B90 B78:B82 B94:B98 B102:B106 B38:B43 B70:B74 E86:E90 E78:E82 E94:E98 E102:E106 E30:E34 E14:E18 E22:E26 E6:E10 E54:E58 E70:E74 E62:E66 E38:E43 E46:E50">
       <formula1>op</formula1>
     </dataValidation>
   </dataValidations>
@@ -4478,27 +4736,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -5744,27 +6002,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -7010,27 +7268,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -8279,27 +8537,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">

</xml_diff>